<commit_message>
Tests (it finally works) and Fixed Sakk(tandem)
</commit_message>
<xml_diff>
--- a/Jelentkezők.xlsx
+++ b/Jelentkezők.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -530,6 +530,573 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gaál Gergely</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>gaalg@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Erőnlét</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gaál Gergely</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>gaalg@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Erőnlét</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Gaál Gergely</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>gaalg@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Erőnlét</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Gaál Gergely</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>gaalg@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Erőnlét</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Gaál Gergely</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>gaalg@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Floorball</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>{'csapattars1': 'Szörényi Zalán András', 'csapattars2': 'Koós Andor'}</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>fiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Gaál Gergely</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>gaalg@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Streetball</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>{'csapattars1': 'Szörényi Zalán András', 'csapattars2': 'Nagy Martin'}</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>fiu</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hugh G. Rection</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>hughg@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Nyek</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Asztalitenisz(forgó)</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Molnár István Ádám</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>molnari@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Erőnlét</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Molnár István Ádám</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>molnari@ffg.hu</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Szkander</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Zalán Szorenyi</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>RubikKockaKirakas</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Zalán Szorenyi</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>RubikKockaKirakas</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Zalán Szorenyi</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>RubikKockaKirakas</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Zalán Szorenyi</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>RubikKockaKirakas</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Zalán Szorenyi</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>RubikKockaKirakas</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Zalán Szorenyi</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>RubikKockaKirakas</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Zalán Szorenyi</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Sakk (Tandem)</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>{'csapattars1': 'teszt'}</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mostl yjust added requirements.txt
</commit_message>
<xml_diff>
--- a/Jelentkezők.xlsx
+++ b/Jelentkezők.xlsx
@@ -445,7 +445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
@@ -1097,6 +1097,43 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Szörényi Zalán András</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>szorenyi.za@gmail.com</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Asztalitenisz(forgó)</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Nincs</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>